<commit_message>
Initial commit of Vendor Dashboard
</commit_message>
<xml_diff>
--- a/VendorSide/vs.xlsx
+++ b/VendorSide/vs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Opulence Dashboards\VendorSide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5B922B-9D4D-46E4-BB7A-85997324A1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0324C587-765B-4C13-AD60-08DDE540E98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
   <si>
     <t>Vendor ID</t>
   </si>
@@ -271,13 +271,211 @@
   </si>
   <si>
     <t>22ABCDE4321F1Z4</t>
+  </si>
+  <si>
+    <t>VEND0001</t>
+  </si>
+  <si>
+    <t>SparkTech Solutions</t>
+  </si>
+  <si>
+    <t>IT Services</t>
+  </si>
+  <si>
+    <t>Neha</t>
+  </si>
+  <si>
+    <t>sparktech@example.com</t>
+  </si>
+  <si>
+    <t>Stationery</t>
+  </si>
+  <si>
+    <t>29ABCDE0001F1Z6</t>
+  </si>
+  <si>
+    <t>VEND0002</t>
+  </si>
+  <si>
+    <t>MegaTools Ltd.</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>megtools@example.com</t>
+  </si>
+  <si>
+    <t>Bolts</t>
+  </si>
+  <si>
+    <t>29ABCDE0002F1Z4</t>
+  </si>
+  <si>
+    <t>Blacklisted</t>
+  </si>
+  <si>
+    <t>VEND0003</t>
+  </si>
+  <si>
+    <t>Green Office Supplies</t>
+  </si>
+  <si>
+    <t>Office Supplies</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>greenoffice@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0003F1Z3</t>
+  </si>
+  <si>
+    <t>VEND0004</t>
+  </si>
+  <si>
+    <t>FastBolt Industries</t>
+  </si>
+  <si>
+    <t>fastbolt@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0004F1Z9</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>VEND0005</t>
+  </si>
+  <si>
+    <t>Hyderabad Hardware</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Amit</t>
+  </si>
+  <si>
+    <t>hhware@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0005F1Z3</t>
+  </si>
+  <si>
+    <t>VEND0006</t>
+  </si>
+  <si>
+    <t>CoreCircuit Electronics</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>corecircuit@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0006F1Z7</t>
+  </si>
+  <si>
+    <t>VEND0007</t>
+  </si>
+  <si>
+    <t>Prime IT Networks</t>
+  </si>
+  <si>
+    <t>primeit@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0007F1Z7</t>
+  </si>
+  <si>
+    <t>VEND0008</t>
+  </si>
+  <si>
+    <t>EcoPower Components</t>
+  </si>
+  <si>
+    <t>ecopower@example.com</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>29ABCDE0008F1Z2</t>
+  </si>
+  <si>
+    <t>VEND0009</t>
+  </si>
+  <si>
+    <t>PaperTrail Enterprises</t>
+  </si>
+  <si>
+    <t>Raj</t>
+  </si>
+  <si>
+    <t>papertrail@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0009F1Z8</t>
+  </si>
+  <si>
+    <t>VEND0010</t>
+  </si>
+  <si>
+    <t>NextGen Hardware</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>nextgen@example.com</t>
+  </si>
+  <si>
+    <t>29ABCDE0010F1Z5</t>
+  </si>
+  <si>
+    <t>₹70,001</t>
+  </si>
+  <si>
+    <t>₹70,002</t>
+  </si>
+  <si>
+    <t>₹70,003</t>
+  </si>
+  <si>
+    <t>₹70,004</t>
+  </si>
+  <si>
+    <t>₹70,005</t>
+  </si>
+  <si>
+    <t>₹70,006</t>
+  </si>
+  <si>
+    <t>₹70,007</t>
+  </si>
+  <si>
+    <t>₹70,008</t>
+  </si>
+  <si>
+    <t>₹70,009</t>
+  </si>
+  <si>
+    <t>₹70,010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +487,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -314,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -330,6 +534,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,20 +822,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y27"/>
+  <dimension ref="A1:Y26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6328125" customWidth="1"/>
+    <col min="3" max="3" width="18.08984375" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
     <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
     <col min="8" max="8" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.6328125" bestFit="1" customWidth="1"/>
@@ -638,9 +850,11 @@
     <col min="18" max="18" width="15.90625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.54296875" customWidth="1"/>
+    <col min="22" max="22" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.36328125" customWidth="1"/>
+    <col min="24" max="24" width="17.7265625" customWidth="1"/>
+    <col min="25" max="25" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -732,8 +946,8 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -747,7 +961,7 @@
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
     </row>
-    <row r="3" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -782,10 +996,10 @@
       <c r="K3" s="2">
         <v>10</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="N3" s="3">
@@ -825,7 +1039,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>38</v>
       </c>
@@ -860,10 +1074,10 @@
       <c r="K4" s="2">
         <v>7</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="7" t="s">
         <v>46</v>
       </c>
       <c r="N4" s="3">
@@ -903,7 +1117,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>50</v>
       </c>
@@ -938,10 +1152,10 @@
       <c r="K5" s="2">
         <v>14</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="7" t="s">
         <v>57</v>
       </c>
       <c r="N5" s="3">
@@ -981,7 +1195,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -1016,10 +1230,10 @@
       <c r="K6" s="2">
         <v>5</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="7" t="s">
         <v>67</v>
       </c>
       <c r="N6" s="3">
@@ -1094,10 +1308,10 @@
       <c r="K7" s="2">
         <v>12</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="7" t="s">
         <v>77</v>
       </c>
       <c r="N7" s="3">
@@ -1137,297 +1351,787 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
+    <row r="8" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="2">
+        <f>91-9816965653</f>
+        <v>-9816965562</v>
+      </c>
+      <c r="H8" s="3">
+        <v>45326</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" s="2">
+        <v>6925</v>
+      </c>
+      <c r="K8" s="2">
+        <v>22</v>
+      </c>
+      <c r="L8" s="7">
+        <v>227786.28</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="N8" s="3">
+        <v>45773</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="2">
+        <v>74.28</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>2.39</v>
+      </c>
+      <c r="R8">
+        <v>5</v>
+      </c>
+      <c r="S8">
+        <v>3.6</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8" t="s">
+        <v>85</v>
+      </c>
+      <c r="V8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W8" s="6">
+        <v>45729</v>
+      </c>
+      <c r="X8" s="6">
+        <v>46158</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="2">
+        <f>91-9351732690</f>
+        <v>-9351732599</v>
+      </c>
+      <c r="H9" s="3">
+        <v>45133</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="2">
+        <v>4448</v>
+      </c>
+      <c r="K9" s="2">
+        <v>26</v>
+      </c>
+      <c r="L9" s="7">
+        <v>546059.86</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="N9" s="3">
+        <v>45809</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P9" s="2">
+        <v>86</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>1.3</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
+        <v>92</v>
+      </c>
+      <c r="V9" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="6">
+        <v>45738</v>
+      </c>
+      <c r="X9" s="6">
+        <v>46052</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="2">
+        <f>91-9678150688</f>
+        <v>-9678150597</v>
+      </c>
+      <c r="H10" s="3">
+        <v>44768</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2555</v>
+      </c>
+      <c r="K10" s="2">
+        <v>8</v>
+      </c>
+      <c r="L10" s="7">
+        <v>741382.17</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="N10" s="3">
+        <v>45817</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P10" s="2">
+        <v>84.22</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
+      <c r="U10" t="s">
+        <v>99</v>
+      </c>
+      <c r="V10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" s="6">
+        <v>45552</v>
+      </c>
+      <c r="X10" s="6">
+        <v>46183</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="2">
+        <f>91-9693867752</f>
+        <v>-9693867661</v>
+      </c>
+      <c r="H11" s="3">
+        <v>43247</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="2">
+        <v>7146</v>
+      </c>
+      <c r="K11" s="2">
+        <v>8</v>
+      </c>
+      <c r="L11" s="7">
+        <v>308179.25</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="N11" s="3">
+        <v>45778</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" s="2">
+        <v>83.08</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>1.6</v>
+      </c>
+      <c r="T11">
+        <v>4</v>
+      </c>
+      <c r="U11" t="s">
+        <v>103</v>
+      </c>
+      <c r="V11" t="s">
+        <v>36</v>
+      </c>
+      <c r="W11" s="6">
+        <v>45706</v>
+      </c>
+      <c r="X11" s="6">
+        <v>45961</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="2">
+        <f>91-9828891720</f>
+        <v>-9828891629</v>
+      </c>
+      <c r="H12" s="3">
+        <v>44323</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="2">
+        <v>5814</v>
+      </c>
+      <c r="K12" s="2">
+        <v>17</v>
+      </c>
+      <c r="L12" s="7">
+        <v>522775.45</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="N12" s="3">
+        <v>45775</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="2">
+        <v>73.14</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>9.01</v>
+      </c>
+      <c r="R12">
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>2.4</v>
+      </c>
+      <c r="T12">
         <v>1</v>
       </c>
-      <c r="N8" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="O8" s="2">
+      <c r="U12" t="s">
+        <v>110</v>
+      </c>
+      <c r="V12" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="6">
+        <v>45757</v>
+      </c>
+      <c r="X12" s="6">
+        <v>45878</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="2">
+        <f>91-9309098286</f>
+        <v>-9309098195</v>
+      </c>
+      <c r="H13" s="3">
+        <v>43246</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="2">
+        <v>7407</v>
+      </c>
+      <c r="K13" s="2">
+        <v>25</v>
+      </c>
+      <c r="L13" s="7">
+        <v>684354</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="N13" s="3">
+        <v>45793</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="2">
+        <v>79.33</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>8.34</v>
+      </c>
+      <c r="R13">
+        <v>4</v>
+      </c>
+      <c r="S13">
+        <v>5</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>115</v>
+      </c>
+      <c r="V13" t="s">
+        <v>36</v>
+      </c>
+      <c r="W13" s="6">
+        <v>45587</v>
+      </c>
+      <c r="X13" s="6">
+        <v>45945</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="2">
+        <f>91-9960486286</f>
+        <v>-9960486195</v>
+      </c>
+      <c r="H14" s="3">
+        <v>43724</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="2">
+        <v>6718</v>
+      </c>
+      <c r="K14" s="2">
+        <v>14</v>
+      </c>
+      <c r="L14" s="7">
+        <v>313077.12</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="N14" s="3">
+        <v>45822</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" s="2">
+        <v>75.75</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>7.62</v>
+      </c>
+      <c r="R14">
+        <v>10</v>
+      </c>
+      <c r="S14">
+        <v>1.2</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>119</v>
+      </c>
+      <c r="V14" t="s">
+        <v>49</v>
+      </c>
+      <c r="W14" s="6">
+        <v>45710</v>
+      </c>
+      <c r="X14" s="6">
+        <v>46111</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G15" s="2">
+        <f>91-9928475634</f>
+        <v>-9928475543</v>
+      </c>
+      <c r="H15" s="3">
+        <v>44579</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4321</v>
+      </c>
+      <c r="K15" s="2">
+        <v>20</v>
+      </c>
+      <c r="L15" s="7">
+        <v>465500.12</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="N15" s="3">
+        <v>45804</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="P15" s="2">
+        <v>90.12</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.21</v>
+      </c>
+      <c r="R15">
         <v>1</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="S15">
+        <v>4.7</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="U15" t="s">
+        <v>124</v>
+      </c>
+      <c r="V15" t="s">
         <v>36</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="W15" s="6">
+        <v>45672</v>
+      </c>
+      <c r="X15" s="6">
+        <v>45992</v>
+      </c>
+      <c r="Y15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2">
+    <row r="16" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="2">
+        <f>91-9974156743</f>
+        <v>-9974156652</v>
+      </c>
+      <c r="H16" s="3">
+        <v>44088</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J16" s="2">
+        <v>3890</v>
+      </c>
+      <c r="K16" s="2">
+        <v>10</v>
+      </c>
+      <c r="L16" s="7">
+        <v>223456.45</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="N16" s="3">
+        <v>45757</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P16" s="2">
+        <v>85.34</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>3.45</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+      <c r="S16">
+        <v>3</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+      <c r="U16" t="s">
+        <v>129</v>
+      </c>
+      <c r="V16" t="s">
+        <v>36</v>
+      </c>
+      <c r="W16" s="6">
+        <v>45789</v>
+      </c>
+      <c r="X16" s="6">
+        <v>46058</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G17" s="2">
+        <f>91-9812347865</f>
+        <v>-9812347774</v>
+      </c>
+      <c r="H17" s="3">
+        <v>43070</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="2">
+        <v>8435</v>
+      </c>
+      <c r="K17" s="2">
+        <v>28</v>
+      </c>
+      <c r="L17" s="7">
+        <v>987654.32</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="N17" s="3">
+        <v>45811</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" s="2">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>6.3</v>
+      </c>
+      <c r="R17">
+        <v>6</v>
+      </c>
+      <c r="S17">
+        <v>2.9</v>
+      </c>
+      <c r="T17">
         <v>2</v>
       </c>
-      <c r="N9" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O9" s="2">
-        <v>2</v>
-      </c>
-      <c r="P9" s="2" t="s">
+      <c r="U17" t="s">
+        <v>134</v>
+      </c>
+      <c r="V17" t="s">
         <v>49</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2">
-        <v>3</v>
-      </c>
-      <c r="N11" s="2">
-        <v>3.8</v>
-      </c>
-      <c r="O11" s="2">
-        <v>3</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2">
-        <v>4</v>
-      </c>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2">
-        <v>4</v>
-      </c>
-      <c r="N13" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="O13" s="2">
-        <v>2</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2">
-        <v>3</v>
-      </c>
-      <c r="N15" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="O15" s="2">
-        <v>3</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2">
-        <v>1</v>
-      </c>
-      <c r="N16" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="O16" s="2">
-        <v>2</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2">
-        <v>0</v>
-      </c>
-      <c r="N17" s="2">
-        <v>5</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="W17" s="6">
+        <v>45616</v>
+      </c>
+      <c r="X17" s="6">
+        <v>45991</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1440,23 +2144,13 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2">
-        <v>2</v>
-      </c>
-      <c r="N18" s="2">
-        <v>4</v>
-      </c>
-      <c r="O18" s="2">
-        <v>2</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1469,23 +2163,13 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2">
-        <v>1</v>
-      </c>
-      <c r="N19" s="2">
-        <v>4.3</v>
-      </c>
-      <c r="O19" s="2">
-        <v>1</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1498,23 +2182,13 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2">
-        <v>3</v>
-      </c>
-      <c r="N20" s="2">
-        <v>3.9</v>
-      </c>
-      <c r="O20" s="2">
-        <v>2</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1527,23 +2201,13 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2">
-        <v>0</v>
-      </c>
-      <c r="N21" s="2">
-        <v>4.8</v>
-      </c>
-      <c r="O21" s="2">
-        <v>0</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1556,23 +2220,13 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2">
-        <v>1</v>
-      </c>
-      <c r="N22" s="2">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="O22" s="2">
-        <v>1</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1585,23 +2239,13 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2">
-        <v>4</v>
-      </c>
-      <c r="N23" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="O23" s="2">
-        <v>3</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1614,23 +2258,13 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="2">
-        <v>2</v>
-      </c>
-      <c r="N24" s="2">
-        <v>4</v>
-      </c>
-      <c r="O24" s="2">
-        <v>2</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1643,23 +2277,13 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="2">
-        <v>0</v>
-      </c>
-      <c r="N25" s="2">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O25" s="2">
-        <v>0</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1672,52 +2296,14 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2">
-        <v>1</v>
-      </c>
-      <c r="N26" s="2">
-        <v>4.2</v>
-      </c>
-      <c r="O26" s="2">
-        <v>1</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2">
-        <v>0</v>
-      </c>
-      <c r="N27" s="2">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="O27" s="2">
-        <v>0</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>